<commit_message>
update breakout PCB's for the 50mO and 60mO resistors. Ordered the missing parts
</commit_message>
<xml_diff>
--- a/self-tuning-buck-converter/design/Part Orders/bom_2.xlsx
+++ b/self-tuning-buck-converter/design/Part Orders/bom_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niels\Desktop\self-tuning-buck-converter\self-tuning-buck-converter\design\Part Orders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC32BA28-FA74-4947-8688-628C2CC02693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3E9207-273F-4413-AC18-0586B3E5A411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2850" yWindow="2565" windowWidth="22020" windowHeight="18390" xr2:uid="{403FB037-D2F8-4122-9342-AD0817903523}"/>
+    <workbookView xWindow="3765" yWindow="1290" windowWidth="22020" windowHeight="19425" xr2:uid="{403FB037-D2F8-4122-9342-AD0817903523}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>Supplier</t>
   </si>
@@ -115,13 +115,31 @@
   </si>
   <si>
     <t>IR2125PBF-ND</t>
+  </si>
+  <si>
+    <t>LD1117V50</t>
+  </si>
+  <si>
+    <t>497-7311-5-ND</t>
+  </si>
+  <si>
+    <t>IC REG LINEAR 5V 800MA TO220AB</t>
+  </si>
+  <si>
+    <t>LM7322QMAX/NOPB</t>
+  </si>
+  <si>
+    <t>296-46308-1-ND</t>
+  </si>
+  <si>
+    <t>IC OPAMP GP 2 CIRCUIT 8SOIC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,16 +155,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -154,14 +185,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFABABAB"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFABABAB"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFABABAB"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFABABAB"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE09F31D-6921-4F0E-B3D8-5173ED49AB92}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,7 +676,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -642,6 +691,40 @@
       </c>
       <c r="E9" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="3">
+        <v>4</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>